<commit_message>
resolved menu master bugs and added user master
</commit_message>
<xml_diff>
--- a/uploads/redeem-details.xlsx
+++ b/uploads/redeem-details.xlsx
@@ -427,13 +427,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>DIWALI50</v>
+        <v>HOLI50</v>
       </c>
       <c r="C2" t="str">
         <v>Unknown</v>
       </c>
       <c r="D2" t="str">
-        <v>8/2/2025, 11:41:13 am</v>
+        <v>8/2/2025, 11:37:42 am</v>
       </c>
       <c r="E2" t="str">
         <v/>
@@ -447,13 +447,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>DIWALI50</v>
+        <v>HOLI50</v>
       </c>
       <c r="C3" t="str">
         <v>Unknown</v>
       </c>
       <c r="D3" t="str">
-        <v>8/2/2025, 11:46:17 am</v>
+        <v>8/2/2025, 11:38:21 am</v>
       </c>
       <c r="E3" t="str">
         <v/>
@@ -467,19 +467,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>DIWALI50</v>
+        <v>HOLI50</v>
       </c>
       <c r="C4" t="str">
-        <v>Unknown</v>
+        <v xml:space="preserve">Karelibagh Branch </v>
       </c>
       <c r="D4" t="str">
-        <v>8/2/2025, 12:32:44 pm</v>
+        <v>8/2/2025, 3:02:38 pm</v>
       </c>
       <c r="E4" t="str">
-        <v>ansh</v>
+        <v>Dev</v>
       </c>
       <c r="F4" t="str">
-        <v>9824409782</v>
+        <v>9898561251</v>
       </c>
     </row>
     <row r="5">
@@ -487,19 +487,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>DIWALI50</v>
+        <v>HOLI50</v>
       </c>
       <c r="C5" t="str">
-        <v>Unknown</v>
+        <v xml:space="preserve">Karelibagh Branch </v>
       </c>
       <c r="D5" t="str">
-        <v>8/2/2025, 12:44:31 pm</v>
+        <v>8/2/2025, 3:03:07 pm</v>
       </c>
       <c r="E5" t="str">
-        <v>poojan</v>
+        <v>Poojan</v>
       </c>
       <c r="F5" t="str">
-        <v>9824409782</v>
+        <v>8160754098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>